<commit_message>
Shipping search optimization / verification added
</commit_message>
<xml_diff>
--- a/Ship-Invoice-02282019.xlsx
+++ b/Ship-Invoice-02282019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Computer\Desktop\WestSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DB9AEF-ADA7-441E-93AE-3E269F2E0725}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34084DDA-54C5-4490-A093-96A077E3945C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28305" yWindow="675" windowWidth="27555" windowHeight="6480" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QuoteCal" sheetId="1" state="hidden" r:id="rId1"/>
@@ -925,7 +925,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10031" uniqueCount="5981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10034" uniqueCount="5982">
   <si>
     <t>2018 Goal</t>
   </si>
@@ -18877,6 +18877,9 @@
   </si>
   <si>
     <t>Wilkes-Barre, PA 18769-0001</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -33882,8 +33885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T975"/>
   <sheetViews>
-    <sheetView topLeftCell="A922" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M951" sqref="M951"/>
+    <sheetView tabSelected="1" topLeftCell="A701" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B726" sqref="B726"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42572,7 +42575,7 @@
         <v>9.7100000000000009</v>
       </c>
       <c r="O203" s="176">
-        <f t="shared" ref="O203:O234" si="25">M203-N203</f>
+        <f t="shared" ref="O203:O211" si="25">M203-N203</f>
         <v>72.70999999999961</v>
       </c>
       <c r="P203" s="19">
@@ -49006,7 +49009,7 @@
         <v>299.01</v>
       </c>
       <c r="M355" s="175">
-        <f t="shared" ref="M355:M386" si="41">K355-L355</f>
+        <f t="shared" ref="M355:M380" si="41">K355-L355</f>
         <v>114.87</v>
       </c>
       <c r="O355" s="176">
@@ -49758,7 +49761,7 @@
         <v>153.30000000000001</v>
       </c>
       <c r="O372" s="197">
-        <f t="shared" ref="O372:O403" si="44">M372-N372</f>
+        <f t="shared" ref="O372:O380" si="44">M372-N372</f>
         <v>-9.9000000000003752</v>
       </c>
       <c r="P372" s="19">
@@ -51590,7 +51593,7 @@
         <v>8411.2999999999993</v>
       </c>
       <c r="M414" s="175">
-        <f t="shared" ref="M414:M445" si="48">K414-L414</f>
+        <f t="shared" ref="M414:M435" si="48">K414-L414</f>
         <v>196.65999999999985</v>
       </c>
       <c r="N414">
@@ -53497,8 +53500,8 @@
       <c r="A461">
         <v>25</v>
       </c>
-      <c r="B461" s="3">
-        <v>1</v>
+      <c r="B461" s="3" t="s">
+        <v>5981</v>
       </c>
       <c r="E461">
         <v>58</v>
@@ -53887,7 +53890,7 @@
         <v>273</v>
       </c>
       <c r="O469" s="176">
-        <f t="shared" ref="O469:O500" si="53">M469-N469</f>
+        <f t="shared" ref="O469:O494" si="53">M469-N469</f>
         <v>273</v>
       </c>
       <c r="P469" s="19">
@@ -55691,7 +55694,7 @@
         <v>6184.67</v>
       </c>
       <c r="M513" s="175">
-        <f t="shared" ref="M513:M544" si="57">K513-L513</f>
+        <f t="shared" ref="M513:M536" si="57">K513-L513</f>
         <v>91.569999999999709</v>
       </c>
       <c r="P513" s="19">
@@ -56770,6 +56773,9 @@
       <c r="A544">
         <v>5</v>
       </c>
+      <c r="B544" t="s">
+        <v>5981</v>
+      </c>
       <c r="E544">
         <v>27</v>
       </c>
@@ -61362,7 +61368,7 @@
         <v>15984</v>
       </c>
       <c r="M664" s="175">
-        <f t="shared" ref="M664:M695" si="66">K664-L664</f>
+        <f t="shared" ref="M664:M680" si="66">K664-L664</f>
         <v>63.25</v>
       </c>
       <c r="P664" s="19">
@@ -63460,7 +63466,9 @@
       <c r="A725">
         <v>2</v>
       </c>
-      <c r="B725" s="3"/>
+      <c r="B725" s="3" t="s">
+        <v>5981</v>
+      </c>
       <c r="E725">
         <v>43</v>
       </c>
@@ -67380,7 +67388,7 @@
         <v>6321</v>
       </c>
       <c r="M834" s="175">
-        <f t="shared" ref="M834:M865" si="76">K834-L834</f>
+        <f t="shared" ref="M834:M854" si="76">K834-L834</f>
         <v>15.119999999999891</v>
       </c>
       <c r="P834" s="19">
@@ -69265,7 +69273,7 @@
         <v>4928</v>
       </c>
       <c r="M888" s="175">
-        <f t="shared" ref="M888:M919" si="80">K888-L888</f>
+        <f t="shared" ref="M888:M911" si="80">K888-L888</f>
         <v>-145.76000000000022</v>
       </c>
       <c r="P888" s="19">
@@ -72049,7 +72057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:M847"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A848" workbookViewId="0">
+    <sheetView topLeftCell="A698" workbookViewId="0">
       <selection activeCell="G842" sqref="G842:G847"/>
     </sheetView>
   </sheetViews>

</xml_diff>